<commit_message>
[excel-pipeline] hash_id:58f2b56 commit_msg:修改位置数值 ...
</commit_message>
<xml_diff>
--- a/config/excel/CrystalAttRepo.xlsx
+++ b/config/excel/CrystalAttRepo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="24225" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="CrystalAttRepo" sheetId="1" r:id="rId1"/>
@@ -204,9 +204,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -237,8 +237,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,8 +304,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -267,39 +358,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,17 +375,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -334,59 +387,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -409,7 +409,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,175 +583,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,6 +709,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -733,30 +742,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -768,17 +753,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,6 +774,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -809,152 +809,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -976,8 +976,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2188,7 +2186,7 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C31"/>
+      <selection activeCell="D7" sqref="D7:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -2398,7 +2396,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
@@ -2422,7 +2420,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
@@ -2446,7 +2444,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
@@ -2470,7 +2468,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="15">
         <v>0</v>
@@ -2486,800 +2484,800 @@
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:8">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16">
         <v>40</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="15">
+        <v>4</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0</v>
+      </c>
+      <c r="F14" s="15">
+        <v>3059</v>
+      </c>
+      <c r="G14" s="15">
+        <v>3050</v>
+      </c>
+      <c r="H14" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16">
+        <v>41</v>
+      </c>
+      <c r="D15" s="15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0</v>
+      </c>
+      <c r="F15" s="17">
+        <v>3060</v>
+      </c>
+      <c r="G15" s="17">
+        <v>3051</v>
+      </c>
+      <c r="H15" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:8">
+      <c r="A16" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16">
+        <v>42</v>
+      </c>
+      <c r="D16" s="15">
+        <v>4</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0</v>
+      </c>
+      <c r="F16" s="17">
+        <v>3061</v>
+      </c>
+      <c r="G16" s="17">
+        <v>3052</v>
+      </c>
+      <c r="H16" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:8">
+      <c r="A17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="16">
+        <v>43</v>
+      </c>
+      <c r="D17" s="15">
+        <v>4</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="17">
+        <v>3062</v>
+      </c>
+      <c r="G17" s="17">
+        <v>3053</v>
+      </c>
+      <c r="H17" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:8">
+      <c r="A18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="16">
+        <v>44</v>
+      </c>
+      <c r="D18" s="15">
+        <v>4</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
+      <c r="F18" s="17">
+        <v>3063</v>
+      </c>
+      <c r="G18" s="17">
+        <v>3054</v>
+      </c>
+      <c r="H18" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:8">
+      <c r="A19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16">
+        <v>45</v>
+      </c>
+      <c r="D19" s="15">
+        <v>4</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0</v>
+      </c>
+      <c r="F19" s="17">
+        <v>3064</v>
+      </c>
+      <c r="G19" s="17">
+        <v>3055</v>
+      </c>
+      <c r="H19" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:8">
+      <c r="A20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="16">
+        <v>46</v>
+      </c>
+      <c r="D20" s="15">
+        <v>4</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0</v>
+      </c>
+      <c r="F20" s="17">
+        <v>3065</v>
+      </c>
+      <c r="G20" s="17">
+        <v>3056</v>
+      </c>
+      <c r="H20" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:8">
+      <c r="A21" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="16">
+        <v>47</v>
+      </c>
+      <c r="D21" s="15">
+        <v>4</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0</v>
+      </c>
+      <c r="F21" s="17">
+        <v>3066</v>
+      </c>
+      <c r="G21" s="17">
+        <v>3057</v>
+      </c>
+      <c r="H21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:8">
+      <c r="A22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="16">
+        <v>48</v>
+      </c>
+      <c r="D22" s="15">
+        <v>4</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0</v>
+      </c>
+      <c r="F22" s="17">
+        <v>3067</v>
+      </c>
+      <c r="G22" s="17">
+        <v>3058</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:8">
+      <c r="A23" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18">
+        <v>60</v>
+      </c>
+      <c r="D23" s="17">
         <v>5</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E23" s="17">
         <v>0</v>
       </c>
-      <c r="F14" s="17">
-        <v>3059</v>
-      </c>
-      <c r="G14" s="17">
-        <v>3050</v>
-      </c>
-      <c r="H14" s="17">
+      <c r="F23" s="17">
+        <v>3077</v>
+      </c>
+      <c r="G23" s="17">
+        <v>3068</v>
+      </c>
+      <c r="H23" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:8">
-      <c r="A15" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="18">
+    <row r="24" customHeight="1" spans="1:8">
+      <c r="A24" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18">
+        <v>61</v>
+      </c>
+      <c r="D24" s="17">
+        <v>5</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0</v>
+      </c>
+      <c r="F24" s="17">
+        <v>3078</v>
+      </c>
+      <c r="G24" s="17">
+        <v>3069</v>
+      </c>
+      <c r="H24" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:8">
+      <c r="A25" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18">
+        <v>62</v>
+      </c>
+      <c r="D25" s="17">
+        <v>5</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0</v>
+      </c>
+      <c r="F25" s="17">
+        <v>3079</v>
+      </c>
+      <c r="G25" s="17">
+        <v>3070</v>
+      </c>
+      <c r="H25" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:8">
+      <c r="A26" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18">
+        <v>63</v>
+      </c>
+      <c r="D26" s="17">
+        <v>5</v>
+      </c>
+      <c r="E26" s="17">
+        <v>0</v>
+      </c>
+      <c r="F26" s="17">
+        <v>3080</v>
+      </c>
+      <c r="G26" s="17">
+        <v>3071</v>
+      </c>
+      <c r="H26" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:8">
+      <c r="A27" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="19">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18">
+        <v>64</v>
+      </c>
+      <c r="D27" s="17">
         <v>5</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E27" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="19">
-        <v>3060</v>
-      </c>
-      <c r="G15" s="19">
-        <v>3051</v>
-      </c>
-      <c r="H15" s="19">
+      <c r="F27" s="17">
+        <v>3081</v>
+      </c>
+      <c r="G27" s="17">
+        <v>3072</v>
+      </c>
+      <c r="H27" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:8">
-      <c r="A16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="18">
+    <row r="28" customHeight="1" spans="1:8">
+      <c r="A28" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="19">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18">
+        <v>65</v>
+      </c>
+      <c r="D28" s="17">
         <v>5</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E28" s="17">
         <v>0</v>
       </c>
-      <c r="F16" s="19">
-        <v>3061</v>
-      </c>
-      <c r="G16" s="19">
-        <v>3052</v>
-      </c>
-      <c r="H16" s="19">
+      <c r="F28" s="17">
+        <v>3082</v>
+      </c>
+      <c r="G28" s="17">
+        <v>3073</v>
+      </c>
+      <c r="H28" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:8">
-      <c r="A17" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="18">
+    <row r="29" customHeight="1" spans="1:8">
+      <c r="A29" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="19">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18">
+        <v>66</v>
+      </c>
+      <c r="D29" s="17">
         <v>5</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E29" s="17">
         <v>0</v>
       </c>
-      <c r="F17" s="19">
-        <v>3062</v>
-      </c>
-      <c r="G17" s="19">
-        <v>3053</v>
-      </c>
-      <c r="H17" s="19">
+      <c r="F29" s="17">
+        <v>3083</v>
+      </c>
+      <c r="G29" s="17">
+        <v>3074</v>
+      </c>
+      <c r="H29" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:8">
-      <c r="A18" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="18">
+    <row r="30" customHeight="1" spans="1:8">
+      <c r="A30" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="19">
+      <c r="B30" s="17"/>
+      <c r="C30" s="18">
+        <v>67</v>
+      </c>
+      <c r="D30" s="17">
         <v>5</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E30" s="17">
         <v>0</v>
       </c>
-      <c r="F18" s="19">
-        <v>3063</v>
-      </c>
-      <c r="G18" s="19">
-        <v>3054</v>
-      </c>
-      <c r="H18" s="19">
+      <c r="F30" s="17">
+        <v>3084</v>
+      </c>
+      <c r="G30" s="17">
+        <v>3075</v>
+      </c>
+      <c r="H30" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="1:8">
+      <c r="A31" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18">
+        <v>68</v>
+      </c>
+      <c r="D31" s="17">
+        <v>5</v>
+      </c>
+      <c r="E31" s="17">
+        <v>0</v>
+      </c>
+      <c r="F31" s="17">
+        <v>3085</v>
+      </c>
+      <c r="G31" s="17">
+        <v>3076</v>
+      </c>
+      <c r="H31" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:8">
+      <c r="A32" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15">
+        <v>100</v>
+      </c>
+      <c r="D32" s="15">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="15">
+        <v>1</v>
+      </c>
+      <c r="F32" s="17">
+        <v>3200</v>
+      </c>
+      <c r="G32" s="15">
+        <v>-1</v>
+      </c>
+      <c r="H32" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:8">
+      <c r="A33" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17">
+        <v>101</v>
+      </c>
+      <c r="D33" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="17">
+        <v>1</v>
+      </c>
+      <c r="F33" s="17">
+        <v>3201</v>
+      </c>
+      <c r="G33" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H33" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="1:8">
-      <c r="A19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="18">
-        <v>45</v>
-      </c>
-      <c r="D19" s="19">
+    <row r="34" customHeight="1" spans="1:8">
+      <c r="A34" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17">
+        <v>102</v>
+      </c>
+      <c r="D34" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E34" s="17">
+        <v>1</v>
+      </c>
+      <c r="F34" s="17">
+        <v>3202</v>
+      </c>
+      <c r="G34" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H34" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:8">
+      <c r="A35" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17">
+        <v>103</v>
+      </c>
+      <c r="D35" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E35" s="17">
+        <v>1</v>
+      </c>
+      <c r="F35" s="17">
+        <v>3203</v>
+      </c>
+      <c r="G35" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H35" s="17">
         <v>5</v>
       </c>
-      <c r="E19" s="19">
-        <v>0</v>
-      </c>
-      <c r="F19" s="19">
-        <v>3064</v>
-      </c>
-      <c r="G19" s="19">
-        <v>3055</v>
-      </c>
-      <c r="H19" s="19">
+    </row>
+    <row r="36" customHeight="1" spans="1:8">
+      <c r="A36" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17">
+        <v>104</v>
+      </c>
+      <c r="D36" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E36" s="17">
+        <v>1</v>
+      </c>
+      <c r="F36" s="17">
+        <v>3204</v>
+      </c>
+      <c r="G36" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H36" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="1:8">
-      <c r="A20" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18">
-        <v>46</v>
-      </c>
-      <c r="D20" s="19">
+    <row r="37" customHeight="1" spans="1:8">
+      <c r="A37" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17">
+        <v>105</v>
+      </c>
+      <c r="D37" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E37" s="17">
+        <v>1</v>
+      </c>
+      <c r="F37" s="17">
+        <v>3205</v>
+      </c>
+      <c r="G37" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H37" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" customHeight="1" spans="1:8">
+      <c r="A38" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17">
+        <v>106</v>
+      </c>
+      <c r="D38" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E38" s="17">
+        <v>1</v>
+      </c>
+      <c r="F38" s="17">
+        <v>3206</v>
+      </c>
+      <c r="G38" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H38" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" customHeight="1" spans="1:8">
+      <c r="A39" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17">
+        <v>107</v>
+      </c>
+      <c r="D39" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E39" s="17">
+        <v>1</v>
+      </c>
+      <c r="F39" s="17">
+        <v>3207</v>
+      </c>
+      <c r="G39" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H39" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" customHeight="1" spans="1:8">
+      <c r="A40" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17">
+        <v>108</v>
+      </c>
+      <c r="D40" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E40" s="17">
+        <v>1</v>
+      </c>
+      <c r="F40" s="17">
+        <v>3208</v>
+      </c>
+      <c r="G40" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H40" s="17">
         <v>5</v>
       </c>
-      <c r="E20" s="19">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19">
-        <v>3065</v>
-      </c>
-      <c r="G20" s="19">
-        <v>3056</v>
-      </c>
-      <c r="H20" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="1:8">
-      <c r="A21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="18">
-        <v>47</v>
-      </c>
-      <c r="D21" s="19">
+    </row>
+    <row r="41" customHeight="1" spans="1:8">
+      <c r="A41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17">
+        <v>109</v>
+      </c>
+      <c r="D41" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E41" s="17">
+        <v>1</v>
+      </c>
+      <c r="F41" s="17">
+        <v>3209</v>
+      </c>
+      <c r="G41" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H41" s="17">
         <v>5</v>
       </c>
-      <c r="E21" s="19">
-        <v>0</v>
-      </c>
-      <c r="F21" s="19">
-        <v>3066</v>
-      </c>
-      <c r="G21" s="19">
-        <v>3057</v>
-      </c>
-      <c r="H21" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:8">
-      <c r="A22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18">
-        <v>48</v>
-      </c>
-      <c r="D22" s="19">
+    </row>
+    <row r="42" customHeight="1" spans="1:8">
+      <c r="A42" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17">
+        <v>110</v>
+      </c>
+      <c r="D42" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E42" s="17">
+        <v>1</v>
+      </c>
+      <c r="F42" s="17">
+        <v>3210</v>
+      </c>
+      <c r="G42" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H42" s="17">
         <v>5</v>
       </c>
-      <c r="E22" s="19">
-        <v>0</v>
-      </c>
-      <c r="F22" s="19">
-        <v>3067</v>
-      </c>
-      <c r="G22" s="19">
-        <v>3058</v>
-      </c>
-      <c r="H22" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customHeight="1" spans="1:8">
-      <c r="A23" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20">
-        <v>60</v>
-      </c>
-      <c r="D23" s="19">
-        <v>6</v>
-      </c>
-      <c r="E23" s="19">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19">
-        <v>3077</v>
-      </c>
-      <c r="G23" s="19">
-        <v>3068</v>
-      </c>
-      <c r="H23" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" customHeight="1" spans="1:8">
-      <c r="A24" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20">
-        <v>61</v>
-      </c>
-      <c r="D24" s="19">
-        <v>6</v>
-      </c>
-      <c r="E24" s="19">
-        <v>0</v>
-      </c>
-      <c r="F24" s="19">
-        <v>3078</v>
-      </c>
-      <c r="G24" s="19">
-        <v>3069</v>
-      </c>
-      <c r="H24" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" customHeight="1" spans="1:8">
-      <c r="A25" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20">
-        <v>62</v>
-      </c>
-      <c r="D25" s="19">
-        <v>6</v>
-      </c>
-      <c r="E25" s="19">
-        <v>0</v>
-      </c>
-      <c r="F25" s="19">
-        <v>3079</v>
-      </c>
-      <c r="G25" s="19">
-        <v>3070</v>
-      </c>
-      <c r="H25" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" customHeight="1" spans="1:8">
-      <c r="A26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20">
-        <v>63</v>
-      </c>
-      <c r="D26" s="19">
-        <v>6</v>
-      </c>
-      <c r="E26" s="19">
-        <v>0</v>
-      </c>
-      <c r="F26" s="19">
-        <v>3080</v>
-      </c>
-      <c r="G26" s="19">
-        <v>3071</v>
-      </c>
-      <c r="H26" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" customHeight="1" spans="1:8">
-      <c r="A27" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20">
-        <v>64</v>
-      </c>
-      <c r="D27" s="19">
-        <v>6</v>
-      </c>
-      <c r="E27" s="19">
-        <v>0</v>
-      </c>
-      <c r="F27" s="19">
-        <v>3081</v>
-      </c>
-      <c r="G27" s="19">
-        <v>3072</v>
-      </c>
-      <c r="H27" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" customHeight="1" spans="1:8">
-      <c r="A28" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20">
-        <v>65</v>
-      </c>
-      <c r="D28" s="19">
-        <v>6</v>
-      </c>
-      <c r="E28" s="19">
-        <v>0</v>
-      </c>
-      <c r="F28" s="19">
-        <v>3082</v>
-      </c>
-      <c r="G28" s="19">
-        <v>3073</v>
-      </c>
-      <c r="H28" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" customHeight="1" spans="1:8">
-      <c r="A29" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20">
-        <v>66</v>
-      </c>
-      <c r="D29" s="19">
-        <v>6</v>
-      </c>
-      <c r="E29" s="19">
-        <v>0</v>
-      </c>
-      <c r="F29" s="19">
-        <v>3083</v>
-      </c>
-      <c r="G29" s="19">
-        <v>3074</v>
-      </c>
-      <c r="H29" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" customHeight="1" spans="1:8">
-      <c r="A30" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20">
-        <v>67</v>
-      </c>
-      <c r="D30" s="19">
-        <v>6</v>
-      </c>
-      <c r="E30" s="19">
-        <v>0</v>
-      </c>
-      <c r="F30" s="19">
-        <v>3084</v>
-      </c>
-      <c r="G30" s="19">
-        <v>3075</v>
-      </c>
-      <c r="H30" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customHeight="1" spans="1:8">
-      <c r="A31" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20">
-        <v>68</v>
-      </c>
-      <c r="D31" s="19">
-        <v>6</v>
-      </c>
-      <c r="E31" s="19">
-        <v>0</v>
-      </c>
-      <c r="F31" s="19">
-        <v>3085</v>
-      </c>
-      <c r="G31" s="19">
-        <v>3076</v>
-      </c>
-      <c r="H31" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customHeight="1" spans="1:8">
-      <c r="A32" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17">
-        <v>100</v>
-      </c>
-      <c r="D32" s="17">
+    </row>
+    <row r="43" customHeight="1" spans="1:8">
+      <c r="A43" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17">
+        <v>111</v>
+      </c>
+      <c r="D43" s="17">
         <v>-1</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E43" s="17">
         <v>1</v>
       </c>
-      <c r="F32" s="19">
-        <v>3200</v>
-      </c>
-      <c r="G32" s="17">
+      <c r="F43" s="17">
+        <v>3211</v>
+      </c>
+      <c r="G43" s="17">
         <v>-1</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H43" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="33" customHeight="1" spans="1:8">
-      <c r="A33" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19">
-        <v>101</v>
-      </c>
-      <c r="D33" s="19">
+    <row r="44" customHeight="1" spans="1:8">
+      <c r="A44" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17">
+        <v>112</v>
+      </c>
+      <c r="D44" s="17">
         <v>-1</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E44" s="17">
         <v>1</v>
       </c>
-      <c r="F33" s="19">
-        <v>3201</v>
-      </c>
-      <c r="G33" s="19">
+      <c r="F44" s="17">
+        <v>3212</v>
+      </c>
+      <c r="G44" s="17">
         <v>-1</v>
       </c>
-      <c r="H33" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" customHeight="1" spans="1:8">
-      <c r="A34" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19">
-        <v>102</v>
-      </c>
-      <c r="D34" s="19">
+      <c r="H44" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" customHeight="1" spans="1:8">
+      <c r="A45" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17">
+        <v>113</v>
+      </c>
+      <c r="D45" s="17">
         <v>-1</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E45" s="17">
         <v>1</v>
       </c>
-      <c r="F34" s="19">
-        <v>3202</v>
-      </c>
-      <c r="G34" s="19">
+      <c r="F45" s="17">
+        <v>3213</v>
+      </c>
+      <c r="G45" s="17">
         <v>-1</v>
       </c>
-      <c r="H34" s="19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" customHeight="1" spans="1:8">
-      <c r="A35" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19">
-        <v>103</v>
-      </c>
-      <c r="D35" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E35" s="19">
-        <v>1</v>
-      </c>
-      <c r="F35" s="19">
-        <v>3203</v>
-      </c>
-      <c r="G35" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H35" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" customHeight="1" spans="1:8">
-      <c r="A36" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19">
-        <v>104</v>
-      </c>
-      <c r="D36" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E36" s="19">
-        <v>1</v>
-      </c>
-      <c r="F36" s="19">
-        <v>3204</v>
-      </c>
-      <c r="G36" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H36" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" customHeight="1" spans="1:8">
-      <c r="A37" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19">
-        <v>105</v>
-      </c>
-      <c r="D37" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E37" s="19">
-        <v>1</v>
-      </c>
-      <c r="F37" s="19">
-        <v>3205</v>
-      </c>
-      <c r="G37" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H37" s="19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" customHeight="1" spans="1:8">
-      <c r="A38" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19">
-        <v>106</v>
-      </c>
-      <c r="D38" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E38" s="19">
-        <v>1</v>
-      </c>
-      <c r="F38" s="19">
-        <v>3206</v>
-      </c>
-      <c r="G38" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H38" s="19">
+      <c r="H45" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="1:8">
-      <c r="A39" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19">
-        <v>107</v>
-      </c>
-      <c r="D39" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E39" s="19">
-        <v>1</v>
-      </c>
-      <c r="F39" s="19">
-        <v>3207</v>
-      </c>
-      <c r="G39" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H39" s="19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" customHeight="1" spans="1:8">
-      <c r="A40" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19">
-        <v>108</v>
-      </c>
-      <c r="D40" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E40" s="19">
-        <v>1</v>
-      </c>
-      <c r="F40" s="19">
-        <v>3208</v>
-      </c>
-      <c r="G40" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H40" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" customHeight="1" spans="1:8">
-      <c r="A41" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19">
-        <v>109</v>
-      </c>
-      <c r="D41" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E41" s="19">
-        <v>1</v>
-      </c>
-      <c r="F41" s="19">
-        <v>3209</v>
-      </c>
-      <c r="G41" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H41" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" customHeight="1" spans="1:8">
-      <c r="A42" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19">
-        <v>110</v>
-      </c>
-      <c r="D42" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E42" s="19">
-        <v>1</v>
-      </c>
-      <c r="F42" s="19">
-        <v>3210</v>
-      </c>
-      <c r="G42" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H42" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" customHeight="1" spans="1:8">
-      <c r="A43" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19">
-        <v>111</v>
-      </c>
-      <c r="D43" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E43" s="19">
-        <v>1</v>
-      </c>
-      <c r="F43" s="19">
-        <v>3211</v>
-      </c>
-      <c r="G43" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H43" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" customHeight="1" spans="1:8">
-      <c r="A44" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19">
-        <v>112</v>
-      </c>
-      <c r="D44" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E44" s="19">
-        <v>1</v>
-      </c>
-      <c r="F44" s="19">
-        <v>3212</v>
-      </c>
-      <c r="G44" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H44" s="19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" customHeight="1" spans="1:8">
-      <c r="A45" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19">
-        <v>113</v>
-      </c>
-      <c r="D45" s="19">
-        <v>-1</v>
-      </c>
-      <c r="E45" s="19">
-        <v>1</v>
-      </c>
-      <c r="F45" s="19">
-        <v>3213</v>
-      </c>
-      <c r="G45" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H45" s="19">
-        <v>20</v>
-      </c>
-    </row>
     <row r="52" customHeight="1" spans="1:26">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="21"/>
-      <c r="O52" s="21"/>
-      <c r="P52" s="21"/>
-      <c r="Q52" s="21"/>
-      <c r="R52" s="21"/>
-      <c r="S52" s="21"/>
-      <c r="T52" s="21"/>
-      <c r="U52" s="21"/>
-      <c r="V52" s="21"/>
-      <c r="W52" s="21"/>
-      <c r="X52" s="21"/>
-      <c r="Y52" s="21"/>
-      <c r="Z52" s="21"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="19"/>
+      <c r="T52" s="19"/>
+      <c r="U52" s="19"/>
+      <c r="V52" s="19"/>
+      <c r="W52" s="19"/>
+      <c r="X52" s="19"/>
+      <c r="Y52" s="19"/>
+      <c r="Z52" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:518183a commit_msg:修改权重 ...
</commit_message>
<xml_diff>
--- a/config/excel/CrystalAttRepo.xlsx
+++ b/config/excel/CrystalAttRepo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -40,6 +40,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>desc</t>
+  </si>
+  <si>
     <t>pos</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t>导出字段描述</t>
   </si>
   <si>
+    <t>属性描述</t>
+  </si>
+  <si>
     <t>晶石位置</t>
   </si>
   <si>
@@ -80,6 +86,9 @@
   </si>
   <si>
     <t>int32</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
   <si>
     <t>主属性位置1只有攻击力属性</t>
@@ -199,11 +208,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -238,8 +247,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF00B0F0"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -253,7 +271,82 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,97 +360,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -366,8 +368,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,9 +391,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,31 +431,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,7 +467,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,19 +497,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,19 +521,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,18 +569,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -585,6 +581,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -592,12 +600,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,17 +719,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,15 +752,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -771,11 +767,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -803,166 +816,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -991,13 +993,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2200,25 +2196,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A45" sqref="$A45:$XFD45"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5416666666667" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.3083333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.2333333333333" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6166666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54166666666667" style="1" customWidth="1"/>
-    <col min="9" max="16379" width="6" style="1" customWidth="1"/>
-    <col min="16380" max="16384" width="6" style="1"/>
+    <col min="3" max="3" width="10.3083333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.3083333333333" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.2333333333333" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6166666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54166666666667" style="1" customWidth="1"/>
+    <col min="10" max="16380" width="6" style="1" customWidth="1"/>
+    <col min="16381" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customHeight="1" spans="1:8">
+    <row r="1" ht="16.15" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2229,26 +2227,28 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" ht="27" spans="1:8">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" ht="27" spans="1:9">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" ht="14.25" spans="1:8">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" ht="14.25" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -2271,35 +2271,41 @@
       <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:8">
+      <c r="I3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:9">
       <c r="A4" s="3"/>
       <c r="B4" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" spans="1:8">
+        <v>18</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -2307,920 +2313,1035 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-    </row>
-    <row r="6" ht="14.25" spans="1:8">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" ht="14.25" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" ht="13.5" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" spans="1:9">
       <c r="A7" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="13">
-        <v>0</v>
+      <c r="D7" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
         <v>3001</v>
       </c>
-      <c r="G7" s="14">
+      <c r="H7" s="14">
         <v>3000</v>
       </c>
-      <c r="H7" s="14">
+      <c r="I7" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="1:8">
+    <row r="8" customHeight="1" spans="1:9">
       <c r="A8" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13">
         <v>10</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <v>0</v>
       </c>
-      <c r="F8" s="12">
+      <c r="G8" s="12">
         <v>3011</v>
       </c>
-      <c r="G8" s="12">
+      <c r="H8" s="12">
         <v>3010</v>
       </c>
-      <c r="H8" s="14">
+      <c r="I8" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="1:8">
+    <row r="9" customHeight="1" spans="1:9">
       <c r="A9" s="11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13">
         <v>20</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="13">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="F9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="12">
+      <c r="G9" s="12">
         <v>3021</v>
       </c>
-      <c r="G9" s="12">
+      <c r="H9" s="12">
         <v>3020</v>
       </c>
-      <c r="H9" s="14">
+      <c r="I9" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="10" customHeight="1" spans="1:8">
+    <row r="10" customHeight="1" spans="1:9">
       <c r="A10" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13">
         <v>30</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="13">
         <v>3</v>
       </c>
-      <c r="E10" s="12">
+      <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="F10" s="12">
+      <c r="G10" s="12">
         <v>3031</v>
       </c>
-      <c r="G10" s="12">
+      <c r="H10" s="12">
         <v>3030</v>
       </c>
-      <c r="H10" s="12">
+      <c r="I10" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="11" customHeight="1" spans="1:8">
+    <row r="11" customHeight="1" spans="1:9">
       <c r="A11" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13">
         <v>31</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="13">
         <v>3</v>
       </c>
-      <c r="E11" s="12">
+      <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G11" s="12">
         <v>3033</v>
       </c>
-      <c r="G11" s="12">
+      <c r="H11" s="12">
         <v>3032</v>
       </c>
-      <c r="H11" s="12">
+      <c r="I11" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:8">
+    <row r="12" customHeight="1" spans="1:9">
       <c r="A12" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13">
         <v>32</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="13">
         <v>3</v>
       </c>
-      <c r="E12" s="12">
+      <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="F12" s="12">
+      <c r="G12" s="12">
         <v>3035</v>
       </c>
-      <c r="G12" s="12">
+      <c r="H12" s="12">
         <v>3034</v>
       </c>
-      <c r="H12" s="12">
+      <c r="I12" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="1:8">
+    <row r="13" customHeight="1" spans="1:9">
       <c r="A13" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="13">
         <v>33</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="16">
         <v>3</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F13" s="15">
         <v>0</v>
       </c>
-      <c r="F13" s="15">
+      <c r="G13" s="15">
         <v>3037</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H13" s="15">
         <v>3036</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I13" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="1:8">
+    <row r="14" customHeight="1" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16">
         <v>40</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="15">
         <v>4</v>
       </c>
-      <c r="E14" s="15">
+      <c r="F14" s="15">
         <v>0</v>
       </c>
-      <c r="F14" s="15">
+      <c r="G14" s="15">
         <v>3059</v>
       </c>
-      <c r="G14" s="15">
+      <c r="H14" s="15">
         <v>3050</v>
       </c>
-      <c r="H14" s="15">
+      <c r="I14" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:8">
+    <row r="15" customHeight="1" spans="1:9">
       <c r="A15" s="17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="16">
         <v>41</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="15">
         <v>4</v>
       </c>
-      <c r="E15" s="17">
+      <c r="F15" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="17">
+      <c r="G15" s="17">
         <v>3060</v>
       </c>
-      <c r="G15" s="17">
+      <c r="H15" s="17">
         <v>3051</v>
       </c>
-      <c r="H15" s="17">
+      <c r="I15" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:8">
+    <row r="16" customHeight="1" spans="1:9">
       <c r="A16" s="17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="16">
         <v>42</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="15">
         <v>4</v>
       </c>
-      <c r="E16" s="17">
+      <c r="F16" s="17">
         <v>0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="G16" s="17">
         <v>3061</v>
       </c>
-      <c r="G16" s="17">
+      <c r="H16" s="17">
         <v>3052</v>
       </c>
-      <c r="H16" s="17">
+      <c r="I16" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:8">
+    <row r="17" customHeight="1" spans="1:9">
       <c r="A17" s="17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="16">
         <v>43</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="15">
         <v>4</v>
       </c>
-      <c r="E17" s="17">
+      <c r="F17" s="17">
         <v>0</v>
       </c>
-      <c r="F17" s="17">
+      <c r="G17" s="17">
         <v>3062</v>
       </c>
-      <c r="G17" s="17">
+      <c r="H17" s="17">
         <v>3053</v>
       </c>
-      <c r="H17" s="17">
+      <c r="I17" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:8">
+    <row r="18" customHeight="1" spans="1:9">
       <c r="A18" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="16">
         <v>44</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="15">
         <v>4</v>
       </c>
-      <c r="E18" s="17">
+      <c r="F18" s="17">
         <v>0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="G18" s="17">
         <v>3063</v>
       </c>
-      <c r="G18" s="17">
+      <c r="H18" s="17">
         <v>3054</v>
       </c>
-      <c r="H18" s="17">
+      <c r="I18" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="1:8">
+    <row r="19" customHeight="1" spans="1:9">
       <c r="A19" s="17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="16">
         <v>45</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="15">
         <v>4</v>
       </c>
-      <c r="E19" s="17">
+      <c r="F19" s="17">
         <v>0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="G19" s="17">
         <v>3064</v>
       </c>
-      <c r="G19" s="17">
+      <c r="H19" s="17">
         <v>3055</v>
       </c>
-      <c r="H19" s="17">
+      <c r="I19" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="1:8">
+    <row r="20" customHeight="1" spans="1:9">
       <c r="A20" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="16">
         <v>46</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="15">
         <v>4</v>
       </c>
-      <c r="E20" s="17">
+      <c r="F20" s="17">
         <v>0</v>
       </c>
-      <c r="F20" s="17">
+      <c r="G20" s="17">
         <v>3065</v>
       </c>
-      <c r="G20" s="17">
+      <c r="H20" s="17">
         <v>3056</v>
       </c>
-      <c r="H20" s="17">
+      <c r="I20" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="21" customHeight="1" spans="1:8">
+    <row r="21" customHeight="1" spans="1:9">
       <c r="A21" s="17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="16">
         <v>47</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15">
         <v>4</v>
       </c>
-      <c r="E21" s="17">
+      <c r="F21" s="17">
         <v>0</v>
       </c>
-      <c r="F21" s="17">
+      <c r="G21" s="17">
         <v>3066</v>
       </c>
-      <c r="G21" s="17">
+      <c r="H21" s="17">
         <v>3057</v>
       </c>
-      <c r="H21" s="17">
+      <c r="I21" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="22" customHeight="1" spans="1:8">
+    <row r="22" customHeight="1" spans="1:9">
       <c r="A22" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="16">
         <v>48</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="15">
         <v>4</v>
       </c>
-      <c r="E22" s="17">
+      <c r="F22" s="17">
         <v>0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="G22" s="17">
         <v>3067</v>
       </c>
-      <c r="G22" s="17">
+      <c r="H22" s="17">
         <v>3058</v>
       </c>
-      <c r="H22" s="17">
+      <c r="I22" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="1:8">
+    <row r="23" customHeight="1" spans="1:9">
       <c r="A23" s="17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18">
         <v>60</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="17">
         <v>5</v>
       </c>
-      <c r="E23" s="17">
+      <c r="F23" s="17">
         <v>0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="G23" s="17">
         <v>3077</v>
       </c>
-      <c r="G23" s="17">
+      <c r="H23" s="17">
         <v>3068</v>
       </c>
-      <c r="H23" s="17">
+      <c r="I23" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="1:8">
+    <row r="24" customHeight="1" spans="1:9">
       <c r="A24" s="17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="18">
         <v>61</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="17">
         <v>5</v>
       </c>
-      <c r="E24" s="17">
+      <c r="F24" s="17">
         <v>0</v>
       </c>
-      <c r="F24" s="17">
+      <c r="G24" s="17">
         <v>3078</v>
       </c>
-      <c r="G24" s="17">
+      <c r="H24" s="17">
         <v>3069</v>
       </c>
-      <c r="H24" s="17">
+      <c r="I24" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="1:8">
+    <row r="25" customHeight="1" spans="1:9">
       <c r="A25" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="18">
         <v>62</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="17">
         <v>5</v>
       </c>
-      <c r="E25" s="17">
+      <c r="F25" s="17">
         <v>0</v>
       </c>
-      <c r="F25" s="17">
+      <c r="G25" s="17">
         <v>3079</v>
       </c>
-      <c r="G25" s="17">
+      <c r="H25" s="17">
         <v>3070</v>
       </c>
-      <c r="H25" s="17">
+      <c r="I25" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="1:8">
+    <row r="26" customHeight="1" spans="1:9">
       <c r="A26" s="17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="18">
         <v>63</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="17">
         <v>5</v>
       </c>
-      <c r="E26" s="17">
+      <c r="F26" s="17">
         <v>0</v>
       </c>
-      <c r="F26" s="17">
+      <c r="G26" s="17">
         <v>3080</v>
       </c>
-      <c r="G26" s="17">
+      <c r="H26" s="17">
         <v>3071</v>
       </c>
-      <c r="H26" s="17">
+      <c r="I26" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="1:8">
+    <row r="27" customHeight="1" spans="1:9">
       <c r="A27" s="17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="18">
         <v>64</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="17">
         <v>5</v>
       </c>
-      <c r="E27" s="17">
+      <c r="F27" s="17">
         <v>0</v>
       </c>
-      <c r="F27" s="17">
+      <c r="G27" s="17">
         <v>3081</v>
       </c>
-      <c r="G27" s="17">
+      <c r="H27" s="17">
         <v>3072</v>
       </c>
-      <c r="H27" s="17">
+      <c r="I27" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="1:8">
+    <row r="28" customHeight="1" spans="1:9">
       <c r="A28" s="17" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18">
         <v>65</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="17">
         <v>5</v>
       </c>
-      <c r="E28" s="17">
+      <c r="F28" s="17">
         <v>0</v>
       </c>
-      <c r="F28" s="17">
+      <c r="G28" s="17">
         <v>3082</v>
       </c>
-      <c r="G28" s="17">
+      <c r="H28" s="17">
         <v>3073</v>
       </c>
-      <c r="H28" s="17">
+      <c r="I28" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="1:8">
+    <row r="29" customHeight="1" spans="1:9">
       <c r="A29" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18">
         <v>66</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="17">
         <v>5</v>
       </c>
-      <c r="E29" s="17">
+      <c r="F29" s="17">
         <v>0</v>
       </c>
-      <c r="F29" s="17">
+      <c r="G29" s="17">
         <v>3083</v>
       </c>
-      <c r="G29" s="17">
+      <c r="H29" s="17">
         <v>3074</v>
       </c>
-      <c r="H29" s="17">
+      <c r="I29" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="1:8">
+    <row r="30" customHeight="1" spans="1:9">
       <c r="A30" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="18">
         <v>67</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="17">
         <v>5</v>
       </c>
-      <c r="E30" s="17">
+      <c r="F30" s="17">
         <v>0</v>
       </c>
-      <c r="F30" s="17">
+      <c r="G30" s="17">
         <v>3084</v>
       </c>
-      <c r="G30" s="17">
+      <c r="H30" s="17">
         <v>3075</v>
       </c>
-      <c r="H30" s="17">
+      <c r="I30" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="1:8">
+    <row r="31" customHeight="1" spans="1:9">
       <c r="A31" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="18">
         <v>68</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="17">
         <v>5</v>
       </c>
-      <c r="E31" s="17">
+      <c r="F31" s="17">
         <v>0</v>
       </c>
-      <c r="F31" s="17">
+      <c r="G31" s="17">
         <v>3085</v>
       </c>
-      <c r="G31" s="17">
+      <c r="H31" s="17">
         <v>3076</v>
       </c>
-      <c r="H31" s="17">
+      <c r="I31" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="32" customHeight="1" spans="1:8">
+    <row r="32" customHeight="1" spans="1:9">
       <c r="A32" s="15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15">
         <v>100</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="15">
         <v>-1</v>
       </c>
-      <c r="E32" s="15">
+      <c r="F32" s="15">
         <v>1</v>
       </c>
-      <c r="F32" s="17">
+      <c r="G32" s="17">
         <v>3200</v>
       </c>
-      <c r="G32" s="15">
+      <c r="H32" s="15">
         <v>-1</v>
       </c>
-      <c r="H32" s="15">
+      <c r="I32" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="33" customHeight="1" spans="1:8">
+    <row r="33" customHeight="1" spans="1:9">
       <c r="A33" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17">
         <v>101</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="17">
         <v>-1</v>
       </c>
-      <c r="E33" s="17">
+      <c r="F33" s="17">
         <v>1</v>
       </c>
-      <c r="F33" s="17">
+      <c r="G33" s="17">
         <v>3201</v>
       </c>
-      <c r="G33" s="17">
+      <c r="H33" s="17">
         <v>-1</v>
       </c>
-      <c r="H33" s="17">
+      <c r="I33" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="1:8">
+    <row r="34" customHeight="1" spans="1:9">
       <c r="A34" s="17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17">
         <v>102</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="17">
         <v>-1</v>
       </c>
-      <c r="E34" s="17">
+      <c r="F34" s="17">
         <v>1</v>
       </c>
-      <c r="F34" s="17">
+      <c r="G34" s="17">
         <v>3202</v>
       </c>
-      <c r="G34" s="17">
+      <c r="H34" s="17">
         <v>-1</v>
       </c>
-      <c r="H34" s="17">
+      <c r="I34" s="17">
         <v>30</v>
       </c>
     </row>
-    <row r="35" customHeight="1" spans="1:8">
+    <row r="35" customHeight="1" spans="1:9">
       <c r="A35" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17">
         <v>103</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="17">
         <v>-1</v>
       </c>
-      <c r="E35" s="17">
+      <c r="F35" s="17">
         <v>1</v>
       </c>
-      <c r="F35" s="17">
+      <c r="G35" s="17">
         <v>3203</v>
       </c>
-      <c r="G35" s="17">
+      <c r="H35" s="17">
         <v>-1</v>
       </c>
-      <c r="H35" s="17">
+      <c r="I35" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="36" customHeight="1" spans="1:8">
+    <row r="36" customHeight="1" spans="1:9">
       <c r="A36" s="17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17">
         <v>104</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="17">
         <v>-1</v>
       </c>
-      <c r="E36" s="17">
+      <c r="F36" s="17">
         <v>1</v>
       </c>
-      <c r="F36" s="17">
+      <c r="G36" s="17">
         <v>3204</v>
       </c>
-      <c r="G36" s="17">
+      <c r="H36" s="17">
         <v>-1</v>
       </c>
-      <c r="H36" s="17">
+      <c r="I36" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="37" customHeight="1" spans="1:8">
+    <row r="37" customHeight="1" spans="1:9">
       <c r="A37" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17">
         <v>105</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="17">
         <v>-1</v>
       </c>
-      <c r="E37" s="17">
+      <c r="F37" s="17">
         <v>1</v>
       </c>
-      <c r="F37" s="17">
+      <c r="G37" s="17">
         <v>3205</v>
       </c>
-      <c r="G37" s="17">
+      <c r="H37" s="17">
         <v>-1</v>
       </c>
-      <c r="H37" s="17">
+      <c r="I37" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="38" customHeight="1" spans="1:8">
+    <row r="38" customHeight="1" spans="1:9">
       <c r="A38" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17">
         <v>106</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="17">
         <v>-1</v>
       </c>
-      <c r="E38" s="17">
+      <c r="F38" s="17">
         <v>1</v>
       </c>
-      <c r="F38" s="17">
+      <c r="G38" s="17">
         <v>3206</v>
       </c>
-      <c r="G38" s="17">
+      <c r="H38" s="17">
         <v>-1</v>
       </c>
-      <c r="H38" s="17">
+      <c r="I38" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="1:8">
+    <row r="39" customHeight="1" spans="1:9">
       <c r="A39" s="17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17">
         <v>107</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="17">
         <v>-1</v>
       </c>
-      <c r="E39" s="17">
+      <c r="F39" s="17">
         <v>1</v>
       </c>
-      <c r="F39" s="17">
+      <c r="G39" s="17">
         <v>3207</v>
       </c>
-      <c r="G39" s="17">
+      <c r="H39" s="17">
         <v>-1</v>
       </c>
-      <c r="H39" s="17">
+      <c r="I39" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="1:8">
+    <row r="40" customHeight="1" spans="1:9">
       <c r="A40" s="17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17">
         <v>108</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="17">
         <v>-1</v>
       </c>
-      <c r="E40" s="17">
+      <c r="F40" s="17">
         <v>1</v>
       </c>
-      <c r="F40" s="17">
+      <c r="G40" s="17">
         <v>3209</v>
       </c>
-      <c r="G40" s="17">
+      <c r="H40" s="17">
         <v>-1</v>
       </c>
-      <c r="H40" s="17">
+      <c r="I40" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="41" customHeight="1" spans="1:8">
+    <row r="41" customHeight="1" spans="1:9">
       <c r="A41" s="17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17">
         <v>109</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="17">
         <v>-1</v>
       </c>
-      <c r="E41" s="17">
+      <c r="F41" s="17">
         <v>1</v>
       </c>
-      <c r="F41" s="17">
+      <c r="G41" s="17">
         <v>3210</v>
       </c>
-      <c r="G41" s="17">
+      <c r="H41" s="17">
         <v>-1</v>
       </c>
-      <c r="H41" s="17">
+      <c r="I41" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="42" customHeight="1" spans="1:8">
+    <row r="42" customHeight="1" spans="1:9">
       <c r="A42" s="17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17">
         <v>110</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="17">
         <v>-1</v>
       </c>
-      <c r="E42" s="17">
+      <c r="F42" s="17">
         <v>1</v>
       </c>
-      <c r="F42" s="17">
+      <c r="G42" s="17">
         <v>3211</v>
       </c>
-      <c r="G42" s="17">
+      <c r="H42" s="17">
         <v>-1</v>
       </c>
-      <c r="H42" s="17">
+      <c r="I42" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="43" customHeight="1" spans="1:8">
+    <row r="43" customHeight="1" spans="1:9">
       <c r="A43" s="17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17">
         <v>111</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="17">
         <v>-1</v>
       </c>
-      <c r="E43" s="17">
+      <c r="F43" s="17">
         <v>1</v>
       </c>
-      <c r="F43" s="17">
+      <c r="G43" s="17">
         <v>3212</v>
       </c>
-      <c r="G43" s="17">
+      <c r="H43" s="17">
         <v>-1</v>
       </c>
-      <c r="H43" s="17">
+      <c r="I43" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="45" customHeight="1" spans="1:23">
+    <row r="45" customHeight="1" spans="1:24">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
@@ -3240,38 +3361,40 @@
       <c r="Q45" s="19"/>
       <c r="R45" s="19"/>
       <c r="S45" s="19"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="22"/>
-      <c r="V45" s="21"/>
-      <c r="W45" s="22"/>
-    </row>
-    <row r="50" customHeight="1" spans="1:26">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
-      <c r="T50" s="20"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
-      <c r="Z50" s="20"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+    </row>
+    <row r="50" customHeight="1" spans="1:27">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
+      <c r="AA50" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:446f901 commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev
# Conflicts:
#	global/SkillBase.xlsx ...
</commit_message>
<xml_diff>
--- a/config/excel/CrystalAttRepo.xlsx
+++ b/config/excel/CrystalAttRepo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -40,9 +40,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>pos</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>导出字段描述</t>
   </si>
   <si>
-    <t>属性描述</t>
-  </si>
-  <si>
     <t>晶石位置</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>int32</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>主属性位置1只有攻击力属性</t>
   </si>
   <si>
@@ -184,22 +175,28 @@
     <t>副属性百分比生命值</t>
   </si>
   <si>
-    <t>副属性百分比治疗量</t>
+    <t>副属性效果命中</t>
   </si>
   <si>
     <t>副属性效果抵抗</t>
   </si>
   <si>
+    <t>副属性总伤害加成</t>
+  </si>
+  <si>
     <t>副属性暴击值</t>
   </si>
   <si>
     <t>副属性暴击倍数</t>
   </si>
   <si>
-    <t>副属性百分比回怒</t>
-  </si>
-  <si>
-    <t>副属性百分比MP恢复</t>
+    <t>副属性百分比时速</t>
+  </si>
+  <si>
+    <t>副属性百分比移速</t>
+  </si>
+  <si>
+    <t>副属性治疗量</t>
   </si>
 </sst>
 </file>
@@ -207,12 +204,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -240,10 +237,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF00B0F0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -255,11 +253,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,13 +271,6 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -291,31 +288,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,14 +312,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
@@ -360,9 +327,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,10 +367,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -392,7 +382,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,7 +409,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,13 +469,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,19 +487,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,108 +571,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -587,19 +583,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,15 +718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -752,17 +733,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -778,17 +753,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,6 +774,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -819,152 +809,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -991,9 +981,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2196,27 +2183,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D7" sqref="D7:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5416666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3083333333333" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.3083333333333" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.2333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6166666666667" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.54166666666667" style="1" customWidth="1"/>
-    <col min="10" max="16380" width="6" style="1" customWidth="1"/>
-    <col min="16381" max="16384" width="6" style="1"/>
+    <col min="3" max="5" width="10.3083333333333" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.2333333333333" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6166666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54166666666667" style="1" customWidth="1"/>
+    <col min="9" max="16379" width="6" style="1" customWidth="1"/>
+    <col min="16380" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customHeight="1" spans="1:9">
+    <row r="1" ht="16.15" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2227,28 +2212,26 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" ht="27" spans="1:9">
+    </row>
+    <row r="2" ht="27" spans="1:8">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" ht="14.25" spans="1:9">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" ht="14.25" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -2271,41 +2254,35 @@
       <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:9">
+    </row>
+    <row r="4" ht="14.25" spans="1:8">
       <c r="A4" s="3"/>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" spans="1:9">
+    </row>
+    <row r="5" ht="14.25" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -2313,1088 +2290,994 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" ht="14.25" spans="1:9">
+    </row>
+    <row r="6" ht="14.25" spans="1:8">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" spans="1:8">
+      <c r="A7" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" ht="13.5" spans="1:9">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>24</v>
+      <c r="D7" s="13">
+        <v>0</v>
       </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="13">
-        <v>0</v>
+      <c r="F7" s="14">
+        <v>3001</v>
       </c>
       <c r="G7" s="14">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="H7" s="14">
-        <v>3000</v>
-      </c>
-      <c r="I7" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="1:9">
+    <row r="8" customHeight="1" spans="1:8">
       <c r="A8" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13">
         <v>10</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>25</v>
+      <c r="D8" s="13">
+        <v>1</v>
       </c>
       <c r="E8" s="13">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13">
         <v>0</v>
       </c>
+      <c r="F8" s="12">
+        <v>3011</v>
+      </c>
       <c r="G8" s="12">
-        <v>3011</v>
-      </c>
-      <c r="H8" s="12">
         <v>3010</v>
       </c>
-      <c r="I8" s="14">
+      <c r="H8" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="1:9">
+    <row r="9" customHeight="1" spans="1:8">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13">
         <v>20</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>26</v>
+      <c r="D9" s="13">
+        <v>2</v>
       </c>
       <c r="E9" s="13">
-        <v>2</v>
-      </c>
-      <c r="F9" s="13">
         <v>0</v>
       </c>
+      <c r="F9" s="12">
+        <v>3021</v>
+      </c>
       <c r="G9" s="12">
-        <v>3021</v>
-      </c>
-      <c r="H9" s="12">
         <v>3020</v>
       </c>
-      <c r="I9" s="14">
+      <c r="H9" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="10" customHeight="1" spans="1:9">
+    <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13">
         <v>30</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="D10" s="13">
         <v>3</v>
       </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
       <c r="F10" s="12">
-        <v>0</v>
+        <v>3031</v>
       </c>
       <c r="G10" s="12">
-        <v>3031</v>
+        <v>3030</v>
       </c>
       <c r="H10" s="12">
-        <v>3030</v>
-      </c>
-      <c r="I10" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="11" customHeight="1" spans="1:9">
+    <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13">
         <v>31</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="D11" s="13">
         <v>3</v>
       </c>
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
       <c r="F11" s="12">
-        <v>0</v>
+        <v>3033</v>
       </c>
       <c r="G11" s="12">
-        <v>3033</v>
+        <v>3032</v>
       </c>
       <c r="H11" s="12">
-        <v>3032</v>
-      </c>
-      <c r="I11" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:9">
+    <row r="12" customHeight="1" spans="1:8">
       <c r="A12" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13">
         <v>32</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="D12" s="13">
         <v>3</v>
       </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
       <c r="F12" s="12">
-        <v>0</v>
+        <v>3035</v>
       </c>
       <c r="G12" s="12">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="H12" s="12">
-        <v>3034</v>
-      </c>
-      <c r="I12" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="1:9">
+    <row r="13" customHeight="1" spans="1:8">
       <c r="A13" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="13">
         <v>33</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="16">
+      <c r="D13" s="16">
         <v>3</v>
       </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
       <c r="F13" s="15">
-        <v>0</v>
+        <v>3037</v>
       </c>
       <c r="G13" s="15">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="H13" s="15">
-        <v>3036</v>
-      </c>
-      <c r="I13" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="1:9">
+    <row r="14" customHeight="1" spans="1:8">
       <c r="A14" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16">
         <v>40</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>31</v>
+      <c r="D14" s="15">
+        <v>4</v>
       </c>
       <c r="E14" s="15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14" s="15">
-        <v>0</v>
+        <v>3059</v>
       </c>
       <c r="G14" s="15">
-        <v>3059</v>
+        <v>3050</v>
       </c>
       <c r="H14" s="15">
-        <v>3050</v>
-      </c>
-      <c r="I14" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:9">
+    <row r="15" customHeight="1" spans="1:8">
       <c r="A15" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="16">
         <v>41</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="15">
+      <c r="D15" s="15">
         <v>4</v>
       </c>
+      <c r="E15" s="17">
+        <v>0</v>
+      </c>
       <c r="F15" s="17">
-        <v>0</v>
+        <v>3060</v>
       </c>
       <c r="G15" s="17">
-        <v>3060</v>
+        <v>3051</v>
       </c>
       <c r="H15" s="17">
-        <v>3051</v>
-      </c>
-      <c r="I15" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:9">
+    <row r="16" customHeight="1" spans="1:8">
       <c r="A16" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="16">
         <v>42</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="15">
+      <c r="D16" s="15">
         <v>4</v>
       </c>
+      <c r="E16" s="17">
+        <v>0</v>
+      </c>
       <c r="F16" s="17">
-        <v>0</v>
+        <v>3061</v>
       </c>
       <c r="G16" s="17">
-        <v>3061</v>
+        <v>3052</v>
       </c>
       <c r="H16" s="17">
-        <v>3052</v>
-      </c>
-      <c r="I16" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:9">
+    <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="16">
         <v>43</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="D17" s="15">
         <v>4</v>
       </c>
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
       <c r="F17" s="17">
-        <v>0</v>
+        <v>3062</v>
       </c>
       <c r="G17" s="17">
-        <v>3062</v>
+        <v>3053</v>
       </c>
       <c r="H17" s="17">
-        <v>3053</v>
-      </c>
-      <c r="I17" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:9">
+    <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="16">
         <v>44</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="15">
+      <c r="D18" s="15">
         <v>4</v>
       </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
       <c r="F18" s="17">
-        <v>0</v>
+        <v>3063</v>
       </c>
       <c r="G18" s="17">
-        <v>3063</v>
+        <v>3054</v>
       </c>
       <c r="H18" s="17">
-        <v>3054</v>
-      </c>
-      <c r="I18" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="1:9">
+    <row r="19" customHeight="1" spans="1:8">
       <c r="A19" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="16">
         <v>45</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="15">
+      <c r="D19" s="15">
         <v>4</v>
       </c>
+      <c r="E19" s="17">
+        <v>0</v>
+      </c>
       <c r="F19" s="17">
-        <v>0</v>
+        <v>3064</v>
       </c>
       <c r="G19" s="17">
-        <v>3064</v>
+        <v>3055</v>
       </c>
       <c r="H19" s="17">
-        <v>3055</v>
-      </c>
-      <c r="I19" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="1:9">
+    <row r="20" customHeight="1" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="16">
         <v>46</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="D20" s="15">
         <v>4</v>
       </c>
+      <c r="E20" s="17">
+        <v>0</v>
+      </c>
       <c r="F20" s="17">
-        <v>0</v>
+        <v>3065</v>
       </c>
       <c r="G20" s="17">
-        <v>3065</v>
+        <v>3056</v>
       </c>
       <c r="H20" s="17">
-        <v>3056</v>
-      </c>
-      <c r="I20" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="21" customHeight="1" spans="1:9">
+    <row r="21" customHeight="1" spans="1:8">
       <c r="A21" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="16">
         <v>47</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="D21" s="15">
         <v>4</v>
       </c>
+      <c r="E21" s="17">
+        <v>0</v>
+      </c>
       <c r="F21" s="17">
+        <v>3066</v>
+      </c>
+      <c r="G21" s="17">
+        <v>3057</v>
+      </c>
+      <c r="H21" s="17">
         <v>0</v>
       </c>
-      <c r="G21" s="17">
-        <v>3066</v>
-      </c>
-      <c r="H21" s="17">
-        <v>3057</v>
-      </c>
-      <c r="I21" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:9">
+    </row>
+    <row r="22" customHeight="1" spans="1:8">
       <c r="A22" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="16">
         <v>48</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="15">
+      <c r="D22" s="15">
         <v>4</v>
       </c>
+      <c r="E22" s="17">
+        <v>0</v>
+      </c>
       <c r="F22" s="17">
+        <v>3067</v>
+      </c>
+      <c r="G22" s="17">
+        <v>3058</v>
+      </c>
+      <c r="H22" s="17">
         <v>0</v>
       </c>
-      <c r="G22" s="17">
-        <v>3067</v>
-      </c>
-      <c r="H22" s="17">
-        <v>3058</v>
-      </c>
-      <c r="I22" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customHeight="1" spans="1:9">
+    </row>
+    <row r="23" customHeight="1" spans="1:8">
       <c r="A23" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18">
         <v>60</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>40</v>
+      <c r="D23" s="17">
+        <v>5</v>
       </c>
       <c r="E23" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F23" s="17">
-        <v>0</v>
+        <v>3077</v>
       </c>
       <c r="G23" s="17">
-        <v>3077</v>
+        <v>3068</v>
       </c>
       <c r="H23" s="17">
-        <v>3068</v>
-      </c>
-      <c r="I23" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="1:9">
+    <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="18">
         <v>61</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>41</v>
+      <c r="D24" s="17">
+        <v>5</v>
       </c>
       <c r="E24" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F24" s="17">
-        <v>0</v>
+        <v>3078</v>
       </c>
       <c r="G24" s="17">
-        <v>3078</v>
+        <v>3069</v>
       </c>
       <c r="H24" s="17">
-        <v>3069</v>
-      </c>
-      <c r="I24" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="1:9">
+    <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="18">
         <v>62</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>42</v>
+      <c r="D25" s="17">
+        <v>5</v>
       </c>
       <c r="E25" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F25" s="17">
-        <v>0</v>
+        <v>3079</v>
       </c>
       <c r="G25" s="17">
-        <v>3079</v>
+        <v>3070</v>
       </c>
       <c r="H25" s="17">
-        <v>3070</v>
-      </c>
-      <c r="I25" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="1:9">
+    <row r="26" customHeight="1" spans="1:8">
       <c r="A26" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="18">
         <v>63</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>43</v>
+      <c r="D26" s="17">
+        <v>5</v>
       </c>
       <c r="E26" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F26" s="17">
-        <v>0</v>
+        <v>3080</v>
       </c>
       <c r="G26" s="17">
-        <v>3080</v>
+        <v>3071</v>
       </c>
       <c r="H26" s="17">
-        <v>3071</v>
-      </c>
-      <c r="I26" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="1:9">
+    <row r="27" customHeight="1" spans="1:8">
       <c r="A27" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="18">
         <v>64</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>44</v>
+      <c r="D27" s="17">
+        <v>5</v>
       </c>
       <c r="E27" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F27" s="17">
-        <v>0</v>
+        <v>3081</v>
       </c>
       <c r="G27" s="17">
-        <v>3081</v>
+        <v>3072</v>
       </c>
       <c r="H27" s="17">
-        <v>3072</v>
-      </c>
-      <c r="I27" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="1:9">
+    <row r="28" customHeight="1" spans="1:8">
       <c r="A28" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18">
         <v>65</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>45</v>
+      <c r="D28" s="17">
+        <v>5</v>
       </c>
       <c r="E28" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F28" s="17">
-        <v>0</v>
+        <v>3082</v>
       </c>
       <c r="G28" s="17">
-        <v>3082</v>
+        <v>3073</v>
       </c>
       <c r="H28" s="17">
-        <v>3073</v>
-      </c>
-      <c r="I28" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="1:9">
+    <row r="29" customHeight="1" spans="1:8">
       <c r="A29" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18">
         <v>66</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>46</v>
+      <c r="D29" s="17">
+        <v>5</v>
       </c>
       <c r="E29" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F29" s="17">
-        <v>0</v>
+        <v>3083</v>
       </c>
       <c r="G29" s="17">
-        <v>3083</v>
+        <v>3074</v>
       </c>
       <c r="H29" s="17">
-        <v>3074</v>
-      </c>
-      <c r="I29" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="1:9">
+    <row r="30" customHeight="1" spans="1:8">
       <c r="A30" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="18">
         <v>67</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>47</v>
+      <c r="D30" s="17">
+        <v>5</v>
       </c>
       <c r="E30" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F30" s="17">
+        <v>3084</v>
+      </c>
+      <c r="G30" s="17">
+        <v>3075</v>
+      </c>
+      <c r="H30" s="17">
         <v>0</v>
       </c>
-      <c r="G30" s="17">
-        <v>3084</v>
-      </c>
-      <c r="H30" s="17">
-        <v>3075</v>
-      </c>
-      <c r="I30" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customHeight="1" spans="1:9">
+    </row>
+    <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="18">
         <v>68</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>48</v>
+      <c r="D31" s="17">
+        <v>5</v>
       </c>
       <c r="E31" s="17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F31" s="17">
+        <v>3085</v>
+      </c>
+      <c r="G31" s="17">
+        <v>3076</v>
+      </c>
+      <c r="H31" s="17">
         <v>0</v>
       </c>
-      <c r="G31" s="17">
-        <v>3085</v>
-      </c>
-      <c r="H31" s="17">
-        <v>3076</v>
-      </c>
-      <c r="I31" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customHeight="1" spans="1:9">
+    </row>
+    <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15">
         <v>100</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>49</v>
+      <c r="D32" s="15">
+        <v>-1</v>
       </c>
       <c r="E32" s="15">
+        <v>1</v>
+      </c>
+      <c r="F32" s="17">
+        <v>3200</v>
+      </c>
+      <c r="G32" s="15">
         <v>-1</v>
       </c>
-      <c r="F32" s="15">
-        <v>1</v>
-      </c>
-      <c r="G32" s="17">
-        <v>3200</v>
-      </c>
       <c r="H32" s="15">
-        <v>-1</v>
-      </c>
-      <c r="I32" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" customHeight="1" spans="1:9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:8">
       <c r="A33" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17">
         <v>101</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>50</v>
+      <c r="D33" s="17">
+        <v>-1</v>
       </c>
       <c r="E33" s="17">
+        <v>1</v>
+      </c>
+      <c r="F33" s="17">
+        <v>3201</v>
+      </c>
+      <c r="G33" s="17">
         <v>-1</v>
       </c>
-      <c r="F33" s="17">
-        <v>1</v>
-      </c>
-      <c r="G33" s="17">
-        <v>3201</v>
-      </c>
       <c r="H33" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I33" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="1:9">
+    <row r="34" customHeight="1" spans="1:8">
       <c r="A34" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17">
         <v>102</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>51</v>
+      <c r="D34" s="17">
+        <v>-1</v>
       </c>
       <c r="E34" s="17">
+        <v>1</v>
+      </c>
+      <c r="F34" s="17">
+        <v>3202</v>
+      </c>
+      <c r="G34" s="17">
         <v>-1</v>
       </c>
-      <c r="F34" s="17">
-        <v>1</v>
-      </c>
-      <c r="G34" s="17">
-        <v>3202</v>
-      </c>
       <c r="H34" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I34" s="17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" customHeight="1" spans="1:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:8">
       <c r="A35" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17">
         <v>103</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>52</v>
+      <c r="D35" s="17">
+        <v>-1</v>
       </c>
       <c r="E35" s="17">
+        <v>1</v>
+      </c>
+      <c r="F35" s="17">
+        <v>3203</v>
+      </c>
+      <c r="G35" s="17">
         <v>-1</v>
       </c>
-      <c r="F35" s="17">
-        <v>1</v>
-      </c>
-      <c r="G35" s="17">
-        <v>3203</v>
-      </c>
       <c r="H35" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I35" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="36" customHeight="1" spans="1:9">
+    <row r="36" customHeight="1" spans="1:8">
       <c r="A36" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17">
         <v>104</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>53</v>
+      <c r="D36" s="17">
+        <v>-1</v>
       </c>
       <c r="E36" s="17">
+        <v>1</v>
+      </c>
+      <c r="F36" s="17">
+        <v>3204</v>
+      </c>
+      <c r="G36" s="17">
         <v>-1</v>
       </c>
-      <c r="F36" s="17">
-        <v>1</v>
-      </c>
-      <c r="G36" s="17">
-        <v>3204</v>
-      </c>
       <c r="H36" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I36" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="37" customHeight="1" spans="1:9">
+    <row r="37" customHeight="1" spans="1:8">
       <c r="A37" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17">
         <v>105</v>
       </c>
-      <c r="D37" s="17" t="s">
-        <v>54</v>
+      <c r="D37" s="17">
+        <v>-1</v>
       </c>
       <c r="E37" s="17">
+        <v>1</v>
+      </c>
+      <c r="F37" s="17">
+        <v>3205</v>
+      </c>
+      <c r="G37" s="17">
         <v>-1</v>
       </c>
-      <c r="F37" s="17">
-        <v>1</v>
-      </c>
-      <c r="G37" s="17">
-        <v>3205</v>
-      </c>
       <c r="H37" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I37" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="38" customHeight="1" spans="1:9">
+    <row r="38" customHeight="1" spans="1:8">
       <c r="A38" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17">
         <v>106</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>55</v>
+      <c r="D38" s="17">
+        <v>-1</v>
       </c>
       <c r="E38" s="17">
+        <v>1</v>
+      </c>
+      <c r="F38" s="17">
+        <v>3206</v>
+      </c>
+      <c r="G38" s="17">
         <v>-1</v>
       </c>
-      <c r="F38" s="17">
-        <v>1</v>
-      </c>
-      <c r="G38" s="17">
-        <v>3206</v>
-      </c>
       <c r="H38" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I38" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="1:9">
+    <row r="39" customHeight="1" spans="1:8">
       <c r="A39" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17">
         <v>107</v>
       </c>
-      <c r="D39" s="17" t="s">
-        <v>56</v>
+      <c r="D39" s="17">
+        <v>-1</v>
       </c>
       <c r="E39" s="17">
+        <v>1</v>
+      </c>
+      <c r="F39" s="17">
+        <v>3207</v>
+      </c>
+      <c r="G39" s="17">
         <v>-1</v>
       </c>
-      <c r="F39" s="17">
-        <v>1</v>
-      </c>
-      <c r="G39" s="17">
-        <v>3207</v>
-      </c>
       <c r="H39" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I39" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="1:9">
+    <row r="40" customHeight="1" spans="1:8">
       <c r="A40" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17">
         <v>108</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>57</v>
+      <c r="D40" s="17">
+        <v>-1</v>
       </c>
       <c r="E40" s="17">
+        <v>1</v>
+      </c>
+      <c r="F40" s="17">
+        <v>3208</v>
+      </c>
+      <c r="G40" s="17">
         <v>-1</v>
       </c>
-      <c r="F40" s="17">
-        <v>1</v>
-      </c>
-      <c r="G40" s="17">
-        <v>3209</v>
-      </c>
       <c r="H40" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I40" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" customHeight="1" spans="1:9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customHeight="1" spans="1:8">
       <c r="A41" s="17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17">
         <v>109</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>58</v>
+      <c r="D41" s="17">
+        <v>-1</v>
       </c>
       <c r="E41" s="17">
+        <v>1</v>
+      </c>
+      <c r="F41" s="17">
+        <v>3209</v>
+      </c>
+      <c r="G41" s="17">
         <v>-1</v>
       </c>
-      <c r="F41" s="17">
-        <v>1</v>
-      </c>
-      <c r="G41" s="17">
-        <v>3210</v>
-      </c>
       <c r="H41" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I41" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" customHeight="1" spans="1:9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:8">
       <c r="A42" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17">
         <v>110</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>59</v>
+      <c r="D42" s="17">
+        <v>-1</v>
       </c>
       <c r="E42" s="17">
+        <v>1</v>
+      </c>
+      <c r="F42" s="17">
+        <v>3210</v>
+      </c>
+      <c r="G42" s="17">
         <v>-1</v>
       </c>
-      <c r="F42" s="17">
-        <v>1</v>
-      </c>
-      <c r="G42" s="17">
-        <v>3211</v>
-      </c>
       <c r="H42" s="17">
-        <v>-1</v>
-      </c>
-      <c r="I42" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" customHeight="1" spans="1:9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customHeight="1" spans="1:8">
       <c r="A43" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17">
         <v>111</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>60</v>
+      <c r="D43" s="17">
+        <v>-1</v>
       </c>
       <c r="E43" s="17">
+        <v>1</v>
+      </c>
+      <c r="F43" s="17">
+        <v>3211</v>
+      </c>
+      <c r="G43" s="17">
         <v>-1</v>
       </c>
-      <c r="F43" s="17">
+      <c r="H43" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customHeight="1" spans="1:8">
+      <c r="A44" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17">
+        <v>112</v>
+      </c>
+      <c r="D44" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E44" s="17">
         <v>1</v>
       </c>
-      <c r="G43" s="17">
+      <c r="F44" s="17">
         <v>3212</v>
       </c>
-      <c r="H43" s="17">
+      <c r="G44" s="17">
         <v>-1</v>
       </c>
-      <c r="I43" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" customHeight="1" spans="1:24">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="20"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-    </row>
-    <row r="50" customHeight="1" spans="1:27">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
-      <c r="T50" s="19"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="19"/>
-      <c r="W50" s="19"/>
-      <c r="X50" s="19"/>
-      <c r="Y50" s="19"/>
-      <c r="Z50" s="19"/>
-      <c r="AA50" s="19"/>
+      <c r="H44" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" customHeight="1" spans="1:8">
+      <c r="A45" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17">
+        <v>113</v>
+      </c>
+      <c r="D45" s="17">
+        <v>-1</v>
+      </c>
+      <c r="E45" s="17">
+        <v>1</v>
+      </c>
+      <c r="F45" s="17">
+        <v>3213</v>
+      </c>
+      <c r="G45" s="17">
+        <v>-1</v>
+      </c>
+      <c r="H45" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" customHeight="1" spans="1:26">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="19"/>
+      <c r="T52" s="19"/>
+      <c r="U52" s="19"/>
+      <c r="V52" s="19"/>
+      <c r="W52" s="19"/>
+      <c r="X52" s="19"/>
+      <c r="Y52" s="19"/>
+      <c r="Z52" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:76c2ac4 commit_msg:还原版本 ...
</commit_message>
<xml_diff>
--- a/config/excel/CrystalAttRepo.xlsx
+++ b/config/excel/CrystalAttRepo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -40,6 +40,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>desc</t>
+  </si>
+  <si>
     <t>pos</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t>导出字段描述</t>
   </si>
   <si>
+    <t>属性描述</t>
+  </si>
+  <si>
     <t>晶石位置</t>
   </si>
   <si>
@@ -82,6 +88,9 @@
     <t>int32</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>主属性位置1只有攻击力属性</t>
   </si>
   <si>
@@ -175,28 +184,22 @@
     <t>副属性百分比生命值</t>
   </si>
   <si>
-    <t>副属性效果命中</t>
+    <t>副属性百分比治疗量</t>
   </si>
   <si>
     <t>副属性效果抵抗</t>
   </si>
   <si>
-    <t>副属性总伤害加成</t>
-  </si>
-  <si>
     <t>副属性暴击值</t>
   </si>
   <si>
     <t>副属性暴击倍数</t>
   </si>
   <si>
-    <t>副属性百分比时速</t>
-  </si>
-  <si>
-    <t>副属性百分比移速</t>
-  </si>
-  <si>
-    <t>副属性治疗量</t>
+    <t>副属性百分比回怒</t>
+  </si>
+  <si>
+    <t>副属性百分比MP恢复</t>
   </si>
 </sst>
 </file>
@@ -204,12 +207,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -237,11 +240,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF00B0F0"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -253,17 +255,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -271,6 +267,13 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -288,9 +291,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,6 +337,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
@@ -327,32 +360,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,10 +377,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -382,7 +392,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -409,7 +419,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,19 +443,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,73 +551,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,49 +569,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,13 +587,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,6 +728,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -733,11 +752,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -753,6 +778,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,32 +810,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -809,152 +819,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -981,6 +991,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2183,25 +2196,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z52"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D31"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5416666666667" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.3083333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.2333333333333" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6166666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54166666666667" style="1" customWidth="1"/>
-    <col min="9" max="16379" width="6" style="1" customWidth="1"/>
-    <col min="16380" max="16384" width="6" style="1"/>
+    <col min="3" max="3" width="10.3083333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.3083333333333" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.2333333333333" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6166666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54166666666667" style="1" customWidth="1"/>
+    <col min="10" max="16380" width="6" style="1" customWidth="1"/>
+    <col min="16381" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customHeight="1" spans="1:8">
+    <row r="1" ht="16.15" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2212,26 +2227,28 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" ht="27" spans="1:8">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" ht="27" spans="1:9">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" ht="14.25" spans="1:8">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" ht="14.25" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -2254,35 +2271,41 @@
       <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:8">
+      <c r="I3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:9">
       <c r="A4" s="3"/>
       <c r="B4" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" spans="1:8">
+        <v>18</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -2290,994 +2313,1088 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-    </row>
-    <row r="6" ht="14.25" spans="1:8">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" ht="14.25" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" ht="13.5" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" spans="1:9">
       <c r="A7" s="11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="13">
-        <v>0</v>
+      <c r="D7" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
         <v>3001</v>
       </c>
-      <c r="G7" s="14">
+      <c r="H7" s="14">
         <v>3000</v>
       </c>
-      <c r="H7" s="14">
+      <c r="I7" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="1:8">
+    <row r="8" customHeight="1" spans="1:9">
       <c r="A8" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13">
         <v>10</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <v>0</v>
       </c>
-      <c r="F8" s="12">
+      <c r="G8" s="12">
         <v>3011</v>
       </c>
-      <c r="G8" s="12">
+      <c r="H8" s="12">
         <v>3010</v>
       </c>
-      <c r="H8" s="14">
+      <c r="I8" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="1:8">
+    <row r="9" customHeight="1" spans="1:9">
       <c r="A9" s="11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13">
         <v>20</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="13">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="F9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="12">
+      <c r="G9" s="12">
         <v>3021</v>
       </c>
-      <c r="G9" s="12">
+      <c r="H9" s="12">
         <v>3020</v>
       </c>
-      <c r="H9" s="14">
+      <c r="I9" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="10" customHeight="1" spans="1:8">
+    <row r="10" customHeight="1" spans="1:9">
       <c r="A10" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13">
         <v>30</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="13">
         <v>3</v>
       </c>
-      <c r="E10" s="12">
+      <c r="F10" s="12">
         <v>0</v>
       </c>
-      <c r="F10" s="12">
+      <c r="G10" s="12">
         <v>3031</v>
       </c>
-      <c r="G10" s="12">
+      <c r="H10" s="12">
         <v>3030</v>
       </c>
-      <c r="H10" s="12">
+      <c r="I10" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="11" customHeight="1" spans="1:8">
+    <row r="11" customHeight="1" spans="1:9">
       <c r="A11" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13">
         <v>31</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="13">
         <v>3</v>
       </c>
-      <c r="E11" s="12">
+      <c r="F11" s="12">
         <v>0</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G11" s="12">
         <v>3033</v>
       </c>
-      <c r="G11" s="12">
+      <c r="H11" s="12">
         <v>3032</v>
       </c>
-      <c r="H11" s="12">
+      <c r="I11" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:8">
+    <row r="12" customHeight="1" spans="1:9">
       <c r="A12" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13">
         <v>32</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="13">
         <v>3</v>
       </c>
-      <c r="E12" s="12">
+      <c r="F12" s="12">
         <v>0</v>
       </c>
-      <c r="F12" s="12">
+      <c r="G12" s="12">
         <v>3035</v>
       </c>
-      <c r="G12" s="12">
+      <c r="H12" s="12">
         <v>3034</v>
       </c>
-      <c r="H12" s="12">
+      <c r="I12" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="1:8">
+    <row r="13" customHeight="1" spans="1:9">
       <c r="A13" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="13">
         <v>33</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="16">
         <v>3</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F13" s="15">
         <v>0</v>
       </c>
-      <c r="F13" s="15">
+      <c r="G13" s="15">
         <v>3037</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H13" s="15">
         <v>3036</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I13" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="1:8">
+    <row r="14" customHeight="1" spans="1:9">
       <c r="A14" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16">
         <v>40</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="15">
         <v>4</v>
       </c>
-      <c r="E14" s="15">
+      <c r="F14" s="15">
         <v>0</v>
       </c>
-      <c r="F14" s="15">
+      <c r="G14" s="15">
         <v>3059</v>
       </c>
-      <c r="G14" s="15">
+      <c r="H14" s="15">
         <v>3050</v>
       </c>
-      <c r="H14" s="15">
+      <c r="I14" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:8">
+    <row r="15" customHeight="1" spans="1:9">
       <c r="A15" s="17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="16">
         <v>41</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="15">
         <v>4</v>
       </c>
-      <c r="E15" s="17">
+      <c r="F15" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="17">
+      <c r="G15" s="17">
         <v>3060</v>
       </c>
-      <c r="G15" s="17">
+      <c r="H15" s="17">
         <v>3051</v>
       </c>
-      <c r="H15" s="17">
+      <c r="I15" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:8">
+    <row r="16" customHeight="1" spans="1:9">
       <c r="A16" s="17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="16">
         <v>42</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="15">
         <v>4</v>
       </c>
-      <c r="E16" s="17">
+      <c r="F16" s="17">
         <v>0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="G16" s="17">
         <v>3061</v>
       </c>
-      <c r="G16" s="17">
+      <c r="H16" s="17">
         <v>3052</v>
       </c>
-      <c r="H16" s="17">
+      <c r="I16" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:8">
+    <row r="17" customHeight="1" spans="1:9">
       <c r="A17" s="17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="16">
         <v>43</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="15">
         <v>4</v>
       </c>
-      <c r="E17" s="17">
+      <c r="F17" s="17">
         <v>0</v>
       </c>
-      <c r="F17" s="17">
+      <c r="G17" s="17">
         <v>3062</v>
       </c>
-      <c r="G17" s="17">
+      <c r="H17" s="17">
         <v>3053</v>
       </c>
-      <c r="H17" s="17">
+      <c r="I17" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:8">
+    <row r="18" customHeight="1" spans="1:9">
       <c r="A18" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="16">
         <v>44</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="15">
         <v>4</v>
       </c>
-      <c r="E18" s="17">
+      <c r="F18" s="17">
         <v>0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="G18" s="17">
         <v>3063</v>
       </c>
-      <c r="G18" s="17">
+      <c r="H18" s="17">
         <v>3054</v>
       </c>
-      <c r="H18" s="17">
+      <c r="I18" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="1:8">
+    <row r="19" customHeight="1" spans="1:9">
       <c r="A19" s="17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="16">
         <v>45</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="15">
         <v>4</v>
       </c>
-      <c r="E19" s="17">
+      <c r="F19" s="17">
         <v>0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="G19" s="17">
         <v>3064</v>
       </c>
-      <c r="G19" s="17">
+      <c r="H19" s="17">
         <v>3055</v>
       </c>
-      <c r="H19" s="17">
+      <c r="I19" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="1:8">
+    <row r="20" customHeight="1" spans="1:9">
       <c r="A20" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="16">
         <v>46</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="15">
         <v>4</v>
       </c>
-      <c r="E20" s="17">
+      <c r="F20" s="17">
         <v>0</v>
       </c>
-      <c r="F20" s="17">
+      <c r="G20" s="17">
         <v>3065</v>
       </c>
-      <c r="G20" s="17">
+      <c r="H20" s="17">
         <v>3056</v>
       </c>
-      <c r="H20" s="17">
+      <c r="I20" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="21" customHeight="1" spans="1:8">
+    <row r="21" customHeight="1" spans="1:9">
       <c r="A21" s="17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="16">
         <v>47</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15">
         <v>4</v>
       </c>
-      <c r="E21" s="17">
+      <c r="F21" s="17">
         <v>0</v>
       </c>
-      <c r="F21" s="17">
+      <c r="G21" s="17">
         <v>3066</v>
       </c>
-      <c r="G21" s="17">
+      <c r="H21" s="17">
         <v>3057</v>
       </c>
-      <c r="H21" s="17">
+      <c r="I21" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="22" customHeight="1" spans="1:8">
+    <row r="22" customHeight="1" spans="1:9">
       <c r="A22" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="16">
         <v>48</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="15">
         <v>4</v>
       </c>
-      <c r="E22" s="17">
+      <c r="F22" s="17">
         <v>0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="G22" s="17">
         <v>3067</v>
       </c>
-      <c r="G22" s="17">
+      <c r="H22" s="17">
         <v>3058</v>
       </c>
-      <c r="H22" s="17">
+      <c r="I22" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="1:8">
+    <row r="23" customHeight="1" spans="1:9">
       <c r="A23" s="17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18">
         <v>60</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="17">
         <v>5</v>
       </c>
-      <c r="E23" s="17">
+      <c r="F23" s="17">
         <v>0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="G23" s="17">
         <v>3077</v>
       </c>
-      <c r="G23" s="17">
+      <c r="H23" s="17">
         <v>3068</v>
       </c>
-      <c r="H23" s="17">
+      <c r="I23" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="1:8">
+    <row r="24" customHeight="1" spans="1:9">
       <c r="A24" s="17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="18">
         <v>61</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="17">
         <v>5</v>
       </c>
-      <c r="E24" s="17">
+      <c r="F24" s="17">
         <v>0</v>
       </c>
-      <c r="F24" s="17">
+      <c r="G24" s="17">
         <v>3078</v>
       </c>
-      <c r="G24" s="17">
+      <c r="H24" s="17">
         <v>3069</v>
       </c>
-      <c r="H24" s="17">
+      <c r="I24" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="1:8">
+    <row r="25" customHeight="1" spans="1:9">
       <c r="A25" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="18">
         <v>62</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="17">
         <v>5</v>
       </c>
-      <c r="E25" s="17">
+      <c r="F25" s="17">
         <v>0</v>
       </c>
-      <c r="F25" s="17">
+      <c r="G25" s="17">
         <v>3079</v>
       </c>
-      <c r="G25" s="17">
+      <c r="H25" s="17">
         <v>3070</v>
       </c>
-      <c r="H25" s="17">
+      <c r="I25" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="1:8">
+    <row r="26" customHeight="1" spans="1:9">
       <c r="A26" s="17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="18">
         <v>63</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="17">
         <v>5</v>
       </c>
-      <c r="E26" s="17">
+      <c r="F26" s="17">
         <v>0</v>
       </c>
-      <c r="F26" s="17">
+      <c r="G26" s="17">
         <v>3080</v>
       </c>
-      <c r="G26" s="17">
+      <c r="H26" s="17">
         <v>3071</v>
       </c>
-      <c r="H26" s="17">
+      <c r="I26" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="1:8">
+    <row r="27" customHeight="1" spans="1:9">
       <c r="A27" s="17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="18">
         <v>64</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="17">
         <v>5</v>
       </c>
-      <c r="E27" s="17">
+      <c r="F27" s="17">
         <v>0</v>
       </c>
-      <c r="F27" s="17">
+      <c r="G27" s="17">
         <v>3081</v>
       </c>
-      <c r="G27" s="17">
+      <c r="H27" s="17">
         <v>3072</v>
       </c>
-      <c r="H27" s="17">
+      <c r="I27" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="1:8">
+    <row r="28" customHeight="1" spans="1:9">
       <c r="A28" s="17" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18">
         <v>65</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="17">
         <v>5</v>
       </c>
-      <c r="E28" s="17">
+      <c r="F28" s="17">
         <v>0</v>
       </c>
-      <c r="F28" s="17">
+      <c r="G28" s="17">
         <v>3082</v>
       </c>
-      <c r="G28" s="17">
+      <c r="H28" s="17">
         <v>3073</v>
       </c>
-      <c r="H28" s="17">
+      <c r="I28" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="1:8">
+    <row r="29" customHeight="1" spans="1:9">
       <c r="A29" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18">
         <v>66</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="17">
         <v>5</v>
       </c>
-      <c r="E29" s="17">
+      <c r="F29" s="17">
         <v>0</v>
       </c>
-      <c r="F29" s="17">
+      <c r="G29" s="17">
         <v>3083</v>
       </c>
-      <c r="G29" s="17">
+      <c r="H29" s="17">
         <v>3074</v>
       </c>
-      <c r="H29" s="17">
+      <c r="I29" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="1:8">
+    <row r="30" customHeight="1" spans="1:9">
       <c r="A30" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="18">
         <v>67</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="17">
         <v>5</v>
       </c>
-      <c r="E30" s="17">
+      <c r="F30" s="17">
         <v>0</v>
       </c>
-      <c r="F30" s="17">
+      <c r="G30" s="17">
         <v>3084</v>
       </c>
-      <c r="G30" s="17">
+      <c r="H30" s="17">
         <v>3075</v>
       </c>
-      <c r="H30" s="17">
+      <c r="I30" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="1:8">
+    <row r="31" customHeight="1" spans="1:9">
       <c r="A31" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="18">
         <v>68</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="17">
         <v>5</v>
       </c>
-      <c r="E31" s="17">
+      <c r="F31" s="17">
         <v>0</v>
       </c>
-      <c r="F31" s="17">
+      <c r="G31" s="17">
         <v>3085</v>
       </c>
-      <c r="G31" s="17">
+      <c r="H31" s="17">
         <v>3076</v>
       </c>
-      <c r="H31" s="17">
+      <c r="I31" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="32" customHeight="1" spans="1:8">
+    <row r="32" customHeight="1" spans="1:9">
       <c r="A32" s="15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15">
         <v>100</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="15">
         <v>-1</v>
       </c>
-      <c r="E32" s="15">
+      <c r="F32" s="15">
         <v>1</v>
       </c>
-      <c r="F32" s="17">
+      <c r="G32" s="17">
         <v>3200</v>
       </c>
-      <c r="G32" s="15">
+      <c r="H32" s="15">
         <v>-1</v>
       </c>
-      <c r="H32" s="15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" customHeight="1" spans="1:8">
+      <c r="I32" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:9">
       <c r="A33" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17">
         <v>101</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="17">
         <v>-1</v>
       </c>
-      <c r="E33" s="17">
+      <c r="F33" s="17">
         <v>1</v>
       </c>
-      <c r="F33" s="17">
+      <c r="G33" s="17">
         <v>3201</v>
       </c>
-      <c r="G33" s="17">
+      <c r="H33" s="17">
         <v>-1</v>
       </c>
-      <c r="H33" s="17">
+      <c r="I33" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="1:8">
+    <row r="34" customHeight="1" spans="1:9">
       <c r="A34" s="17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17">
         <v>102</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="17">
         <v>-1</v>
       </c>
-      <c r="E34" s="17">
+      <c r="F34" s="17">
         <v>1</v>
       </c>
-      <c r="F34" s="17">
+      <c r="G34" s="17">
         <v>3202</v>
       </c>
-      <c r="G34" s="17">
+      <c r="H34" s="17">
         <v>-1</v>
       </c>
-      <c r="H34" s="17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" customHeight="1" spans="1:8">
+      <c r="I34" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:9">
       <c r="A35" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17">
         <v>103</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="17">
         <v>-1</v>
       </c>
-      <c r="E35" s="17">
+      <c r="F35" s="17">
         <v>1</v>
       </c>
-      <c r="F35" s="17">
+      <c r="G35" s="17">
         <v>3203</v>
       </c>
-      <c r="G35" s="17">
+      <c r="H35" s="17">
         <v>-1</v>
       </c>
-      <c r="H35" s="17">
+      <c r="I35" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="36" customHeight="1" spans="1:8">
+    <row r="36" customHeight="1" spans="1:9">
       <c r="A36" s="17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17">
         <v>104</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="17">
         <v>-1</v>
       </c>
-      <c r="E36" s="17">
+      <c r="F36" s="17">
         <v>1</v>
       </c>
-      <c r="F36" s="17">
+      <c r="G36" s="17">
         <v>3204</v>
       </c>
-      <c r="G36" s="17">
+      <c r="H36" s="17">
         <v>-1</v>
       </c>
-      <c r="H36" s="17">
+      <c r="I36" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="37" customHeight="1" spans="1:8">
+    <row r="37" customHeight="1" spans="1:9">
       <c r="A37" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17">
         <v>105</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="17">
         <v>-1</v>
       </c>
-      <c r="E37" s="17">
+      <c r="F37" s="17">
         <v>1</v>
       </c>
-      <c r="F37" s="17">
+      <c r="G37" s="17">
         <v>3205</v>
       </c>
-      <c r="G37" s="17">
+      <c r="H37" s="17">
         <v>-1</v>
       </c>
-      <c r="H37" s="17">
+      <c r="I37" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="38" customHeight="1" spans="1:8">
+    <row r="38" customHeight="1" spans="1:9">
       <c r="A38" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17">
         <v>106</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="17">
         <v>-1</v>
       </c>
-      <c r="E38" s="17">
+      <c r="F38" s="17">
         <v>1</v>
       </c>
-      <c r="F38" s="17">
+      <c r="G38" s="17">
         <v>3206</v>
       </c>
-      <c r="G38" s="17">
+      <c r="H38" s="17">
         <v>-1</v>
       </c>
-      <c r="H38" s="17">
+      <c r="I38" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="1:8">
+    <row r="39" customHeight="1" spans="1:9">
       <c r="A39" s="17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17">
         <v>107</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="17">
         <v>-1</v>
       </c>
-      <c r="E39" s="17">
+      <c r="F39" s="17">
         <v>1</v>
       </c>
-      <c r="F39" s="17">
+      <c r="G39" s="17">
         <v>3207</v>
       </c>
-      <c r="G39" s="17">
+      <c r="H39" s="17">
         <v>-1</v>
       </c>
-      <c r="H39" s="17">
+      <c r="I39" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="1:8">
+    <row r="40" customHeight="1" spans="1:9">
       <c r="A40" s="17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17">
         <v>108</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="17">
         <v>-1</v>
       </c>
-      <c r="E40" s="17">
+      <c r="F40" s="17">
         <v>1</v>
       </c>
-      <c r="F40" s="17">
-        <v>3208</v>
-      </c>
       <c r="G40" s="17">
+        <v>3209</v>
+      </c>
+      <c r="H40" s="17">
         <v>-1</v>
       </c>
-      <c r="H40" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" customHeight="1" spans="1:8">
+      <c r="I40" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" customHeight="1" spans="1:9">
       <c r="A41" s="17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17">
         <v>109</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="17">
         <v>-1</v>
       </c>
-      <c r="E41" s="17">
+      <c r="F41" s="17">
         <v>1</v>
       </c>
-      <c r="F41" s="17">
-        <v>3209</v>
-      </c>
       <c r="G41" s="17">
+        <v>3210</v>
+      </c>
+      <c r="H41" s="17">
         <v>-1</v>
       </c>
-      <c r="H41" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" customHeight="1" spans="1:8">
+      <c r="I41" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:9">
       <c r="A42" s="17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17">
         <v>110</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="17">
         <v>-1</v>
       </c>
-      <c r="E42" s="17">
+      <c r="F42" s="17">
         <v>1</v>
       </c>
-      <c r="F42" s="17">
-        <v>3210</v>
-      </c>
       <c r="G42" s="17">
+        <v>3211</v>
+      </c>
+      <c r="H42" s="17">
         <v>-1</v>
       </c>
-      <c r="H42" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" customHeight="1" spans="1:8">
+      <c r="I42" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customHeight="1" spans="1:9">
       <c r="A43" s="17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17">
         <v>111</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="17">
         <v>-1</v>
       </c>
-      <c r="E43" s="17">
+      <c r="F43" s="17">
         <v>1</v>
       </c>
-      <c r="F43" s="17">
-        <v>3211</v>
-      </c>
       <c r="G43" s="17">
+        <v>3212</v>
+      </c>
+      <c r="H43" s="17">
         <v>-1</v>
       </c>
-      <c r="H43" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" customHeight="1" spans="1:8">
-      <c r="A44" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17">
-        <v>112</v>
-      </c>
-      <c r="D44" s="17">
-        <v>-1</v>
-      </c>
-      <c r="E44" s="17">
-        <v>1</v>
-      </c>
-      <c r="F44" s="17">
-        <v>3212</v>
-      </c>
-      <c r="G44" s="17">
-        <v>-1</v>
-      </c>
-      <c r="H44" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" customHeight="1" spans="1:8">
-      <c r="A45" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17">
-        <v>113</v>
-      </c>
-      <c r="D45" s="17">
-        <v>-1</v>
-      </c>
-      <c r="E45" s="17">
-        <v>1</v>
-      </c>
-      <c r="F45" s="17">
-        <v>3213</v>
-      </c>
-      <c r="G45" s="17">
-        <v>-1</v>
-      </c>
-      <c r="H45" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" customHeight="1" spans="1:26">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="19"/>
-      <c r="R52" s="19"/>
-      <c r="S52" s="19"/>
-      <c r="T52" s="19"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="19"/>
-      <c r="W52" s="19"/>
-      <c r="X52" s="19"/>
-      <c r="Y52" s="19"/>
-      <c r="Z52" s="19"/>
+      <c r="I43" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" customHeight="1" spans="1:24">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+    </row>
+    <row r="50" customHeight="1" spans="1:27">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
+      <c r="AA50" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>